<commit_message>
Update of excelfiles to csv files UTF 8 FORMAT
I changed all the excelfiles to CSV UTF 8 FORMAT
</commit_message>
<xml_diff>
--- a/North_Side_A_distrikt/point26/point26_125_2.xlsx
+++ b/North_Side_A_distrikt/point26/point26_125_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikl\Desktop\Quarter på Sanct Croix\Matrikel for North Side A kvarter\Point 27\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikl\Documents\GitHub\Sankt-croix-Anno-1799\North_Side_A_distrikt\point26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EDD5B3B-88C1-4025-B27E-BC097DE4D34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB95CBD1-CA8B-4B29-9B07-AA0521E15C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FF75B95-9441-44C6-8998-AE421EF2B837}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4FF75B95-9441-44C6-8998-AE421EF2B837}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -962,7 +962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -970,10 +970,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -985,10 +985,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1323,59 +1322,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACC1DC3-309D-4BBB-A889-BC6BB1D22CFB}">
-  <dimension ref="A2:L119"/>
+  <dimension ref="B2:I118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="3" max="3" width="29.26953125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.453125" customWidth="1"/>
+    <col min="9" max="9" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="72" customHeight="1">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="2:9" ht="72" customHeight="1">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="2:9" ht="180" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1386,666 +1385,666 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" ht="108" customHeight="1">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="108" customHeight="1">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="108" customHeight="1">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="108" customHeight="1">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="108" customHeight="1">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="180" customHeight="1">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="108" customHeight="1">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="2:9" ht="108" customHeight="1">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="2:9" ht="108" customHeight="1">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:9" ht="108" customHeight="1">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:9" ht="108" customHeight="1">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="2:9" ht="108" customHeight="1">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" ht="108" customHeight="1">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" ht="108" customHeight="1">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" ht="108" customHeight="1">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" ht="108" customHeight="1">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" ht="180" customHeight="1">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" ht="108" customHeight="1">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" ht="180" customHeight="1">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" ht="108" customHeight="1">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" ht="108" customHeight="1">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" ht="252" customHeight="1">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" ht="108" customHeight="1">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="2:9" ht="72" customHeight="1">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" ht="108" customHeight="1">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="2:9" ht="108" customHeight="1">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
     <row r="31" spans="2:9" ht="108" customHeight="1">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>205</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
     </row>
     <row r="32" spans="2:9" ht="108" customHeight="1">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" spans="2:9" ht="108" customHeight="1">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
     </row>
     <row r="34" spans="2:9" ht="108" customHeight="1">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F34" s="1"/>
@@ -2054,16 +2053,16 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="2:9" ht="108" customHeight="1">
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F35" s="1"/>
@@ -2072,16 +2071,16 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="2:9" ht="108" customHeight="1">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F36" s="1"/>
@@ -2090,16 +2089,16 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="2:9" ht="180" customHeight="1">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F37" s="1"/>
@@ -2108,16 +2107,16 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="2:9" ht="108" customHeight="1">
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F38" s="1"/>
@@ -2126,16 +2125,16 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="2:9" ht="144" customHeight="1">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F39" s="1"/>
@@ -2146,16 +2145,16 @@
       <c r="I39" s="7"/>
     </row>
     <row r="40" spans="2:9" ht="108" customHeight="1">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F40" s="1"/>
@@ -2166,16 +2165,16 @@
       <c r="I40" s="7"/>
     </row>
     <row r="41" spans="2:9" ht="216" customHeight="1">
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F41" s="1"/>
@@ -2186,16 +2185,16 @@
       <c r="I41" s="7"/>
     </row>
     <row r="42" spans="2:9" ht="144" customHeight="1">
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F42" s="1"/>
@@ -2206,16 +2205,16 @@
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="2:9" ht="144" customHeight="1">
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F43" s="1"/>
@@ -2226,16 +2225,16 @@
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="2:9" ht="72" customHeight="1">
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="3"/>
       <c r="F44" s="1"/>
       <c r="G44" s="5" t="s">
         <v>259</v>
@@ -2244,16 +2243,16 @@
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="2:9" ht="108" customHeight="1">
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="3"/>
       <c r="F45" s="1"/>
       <c r="G45" s="5" t="s">
         <v>260</v>
@@ -2262,16 +2261,16 @@
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="2:9" ht="72" customHeight="1">
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E46" s="4"/>
+      <c r="E46" s="3"/>
       <c r="F46" s="1"/>
       <c r="G46" s="5" t="s">
         <v>261</v>
@@ -2280,16 +2279,16 @@
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="2:9" ht="108" customHeight="1">
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="3"/>
       <c r="F47" s="1"/>
       <c r="G47" s="5" t="s">
         <v>262</v>
@@ -2298,16 +2297,16 @@
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="2:9" ht="108" customHeight="1">
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E48" s="4"/>
+      <c r="E48" s="3"/>
       <c r="F48" s="1"/>
       <c r="G48" s="5" t="s">
         <v>263</v>
@@ -2316,16 +2315,16 @@
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="2:9" ht="108" customHeight="1">
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E49" s="4"/>
+      <c r="E49" s="3"/>
       <c r="F49" s="1"/>
       <c r="G49" s="5" t="s">
         <v>264</v>
@@ -2334,16 +2333,16 @@
       <c r="I49" s="7"/>
     </row>
     <row r="50" spans="2:9" ht="108" customHeight="1">
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="3"/>
       <c r="F50" s="1"/>
       <c r="G50" s="5" t="s">
         <v>265</v>
@@ -2352,14 +2351,14 @@
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="2:9" ht="72" customHeight="1">
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
       <c r="F51" s="1"/>
       <c r="G51" s="5" t="s">
         <v>266</v>
@@ -2369,11 +2368,11 @@
     </row>
     <row r="52" spans="2:9" ht="72" customHeight="1">
       <c r="B52" s="1"/>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
       <c r="F52" s="1"/>
       <c r="G52" s="5" t="s">
         <v>275</v>
@@ -2382,11 +2381,11 @@
       <c r="I52" s="7"/>
     </row>
     <row r="53" spans="2:9" ht="36" customHeight="1">
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
       <c r="G53" s="5" t="s">
         <v>267</v>
       </c>
@@ -2394,11 +2393,11 @@
       <c r="I53" s="7"/>
     </row>
     <row r="54" spans="2:9" ht="36" customHeight="1">
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
       <c r="G54" s="5" t="s">
         <v>268</v>
       </c>
@@ -2406,11 +2405,11 @@
       <c r="I54" s="7"/>
     </row>
     <row r="55" spans="2:9" ht="36" customHeight="1">
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
       <c r="G55" s="5" t="s">
         <v>269</v>
       </c>
@@ -2418,11 +2417,11 @@
       <c r="I55" s="7"/>
     </row>
     <row r="56" spans="2:9" ht="36" customHeight="1">
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
       <c r="G56" s="5" t="s">
         <v>270</v>
       </c>
@@ -2430,9 +2429,9 @@
       <c r="I56" s="7"/>
     </row>
     <row r="57" spans="2:9" ht="36" customHeight="1">
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
       <c r="G57" s="5" t="s">
         <v>271</v>
       </c>
@@ -2440,9 +2439,9 @@
       <c r="I57" s="7"/>
     </row>
     <row r="58" spans="2:9" ht="36" customHeight="1">
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
       <c r="G58" s="5" t="s">
         <v>272</v>
       </c>
@@ -2450,9 +2449,9 @@
       <c r="I58" s="7"/>
     </row>
     <row r="59" spans="2:9" ht="36" customHeight="1">
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
       <c r="G59" s="5" t="s">
         <v>273</v>
       </c>
@@ -2460,682 +2459,410 @@
       <c r="I59" s="7"/>
     </row>
     <row r="60" spans="2:9" ht="36" customHeight="1">
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
       <c r="G60" s="5" t="s">
         <v>274</v>
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="2:9" ht="18">
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="2:9" ht="18">
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-    </row>
-    <row r="63" spans="2:9" ht="18">
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-    </row>
-    <row r="64" spans="2:9" ht="18">
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-    </row>
-    <row r="65" spans="1:12" ht="18">
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-    </row>
-    <row r="66" spans="1:12" ht="18">
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-    </row>
-    <row r="67" spans="1:12" ht="18">
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" spans="1:12" ht="18">
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-    </row>
-    <row r="69" spans="1:12" ht="18">
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-    </row>
-    <row r="70" spans="1:12" ht="18">
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-    </row>
-    <row r="71" spans="1:12" ht="18">
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-    </row>
-    <row r="72" spans="1:12" ht="18">
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-    </row>
-    <row r="73" spans="1:12" ht="18">
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-    </row>
-    <row r="74" spans="1:12" ht="18">
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-    </row>
-    <row r="75" spans="1:12" ht="18">
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-    </row>
-    <row r="76" spans="1:12" ht="18">
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-    </row>
-    <row r="77" spans="1:12" ht="18">
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-    </row>
-    <row r="78" spans="1:12" ht="18">
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-    </row>
-    <row r="79" spans="1:12" ht="18">
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-    </row>
-    <row r="80" spans="1:12" ht="18">
-      <c r="A80" s="9"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="9"/>
-      <c r="J80" s="9"/>
-      <c r="K80" s="9"/>
-      <c r="L80" s="9"/>
-    </row>
-    <row r="81" spans="1:12" ht="18">
-      <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
-      <c r="K81" s="9"/>
-      <c r="L81" s="9"/>
-    </row>
-    <row r="82" spans="1:12" ht="18">
-      <c r="A82" s="9"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="9"/>
-      <c r="K82" s="9"/>
-      <c r="L82" s="9"/>
-    </row>
-    <row r="83" spans="1:12" ht="18">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8"/>
-      <c r="J83" s="9"/>
-      <c r="K83" s="9"/>
-      <c r="L83" s="9"/>
-    </row>
-    <row r="84" spans="1:12" ht="18">
-      <c r="A84" s="9"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="9"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-    </row>
-    <row r="85" spans="1:12" ht="18">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="9"/>
-      <c r="K85" s="9"/>
-      <c r="L85" s="9"/>
-    </row>
-    <row r="86" spans="1:12" ht="18">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="9"/>
-      <c r="K86" s="9"/>
-      <c r="L86" s="9"/>
-    </row>
-    <row r="87" spans="1:12" ht="18">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
-      <c r="I87" s="8"/>
-      <c r="J87" s="9"/>
-      <c r="K87" s="9"/>
-      <c r="L87" s="9"/>
-    </row>
-    <row r="88" spans="1:12" ht="18">
-      <c r="A88" s="9"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="9"/>
-      <c r="K88" s="9"/>
-      <c r="L88" s="9"/>
-    </row>
-    <row r="89" spans="1:12" ht="18">
-      <c r="A89" s="9"/>
-      <c r="B89" s="9"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="9"/>
-      <c r="K89" s="9"/>
-      <c r="L89" s="9"/>
-    </row>
-    <row r="90" spans="1:12" ht="18">
-      <c r="A90" s="9"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8"/>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
-      <c r="L90" s="9"/>
-    </row>
-    <row r="91" spans="1:12" ht="18">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="9"/>
-      <c r="K91" s="9"/>
-      <c r="L91" s="9"/>
-    </row>
-    <row r="92" spans="1:12" ht="18">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="9"/>
-      <c r="K92" s="9"/>
-      <c r="L92" s="9"/>
-    </row>
-    <row r="93" spans="1:12" ht="18">
-      <c r="A93" s="9"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
-      <c r="L93" s="9"/>
-    </row>
-    <row r="94" spans="1:12" ht="18">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="9"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="9"/>
-    </row>
-    <row r="95" spans="1:12" ht="18">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="9"/>
-    </row>
-    <row r="96" spans="1:12" ht="18">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="9"/>
-      <c r="K96" s="9"/>
-      <c r="L96" s="9"/>
-    </row>
-    <row r="97" spans="1:12" ht="108" customHeight="1">
-      <c r="A97" s="9"/>
-      <c r="B97" s="9"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="9"/>
-      <c r="H97" s="9"/>
-      <c r="I97" s="9"/>
-      <c r="J97" s="9"/>
-      <c r="K97" s="9"/>
-      <c r="L97" s="9"/>
-    </row>
-    <row r="98" spans="1:12" ht="18">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="9"/>
-      <c r="H98" s="9"/>
-      <c r="I98" s="9"/>
-      <c r="J98" s="9"/>
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
-    </row>
-    <row r="99" spans="1:12" ht="18">
-      <c r="A99" s="9"/>
-      <c r="B99" s="9"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="9"/>
-      <c r="J99" s="9"/>
-      <c r="K99" s="9"/>
-      <c r="L99" s="9"/>
-    </row>
-    <row r="100" spans="1:12" ht="36" customHeight="1">
-      <c r="A100" s="9"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="9"/>
-      <c r="H100" s="9"/>
-      <c r="I100" s="9"/>
-      <c r="J100" s="9"/>
-      <c r="K100" s="9"/>
-      <c r="L100" s="9"/>
-    </row>
-    <row r="101" spans="1:12" ht="72" customHeight="1">
-      <c r="A101" s="9"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="9"/>
-      <c r="I101" s="9"/>
-      <c r="J101" s="9"/>
-      <c r="K101" s="9"/>
-      <c r="L101" s="9"/>
-    </row>
-    <row r="102" spans="1:12" ht="72" customHeight="1">
-      <c r="A102" s="9"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="9"/>
-      <c r="I102" s="9"/>
-      <c r="J102" s="9"/>
-      <c r="K102" s="9"/>
-      <c r="L102" s="9"/>
-    </row>
-    <row r="103" spans="1:12" ht="36" customHeight="1">
-      <c r="A103" s="9"/>
-      <c r="B103" s="8"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="9"/>
-      <c r="H103" s="9"/>
-      <c r="I103" s="9"/>
-      <c r="J103" s="9"/>
-      <c r="K103" s="9"/>
-      <c r="L103" s="9"/>
-    </row>
-    <row r="104" spans="1:12" ht="72" customHeight="1">
-      <c r="A104" s="9"/>
-      <c r="B104" s="8"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="9"/>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-    </row>
-    <row r="105" spans="1:12" ht="36" customHeight="1">
-      <c r="A105" s="9"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="8"/>
-      <c r="G105" s="9"/>
-      <c r="H105" s="9"/>
-      <c r="I105" s="9"/>
-      <c r="J105" s="9"/>
-      <c r="K105" s="9"/>
-      <c r="L105" s="9"/>
-    </row>
-    <row r="106" spans="1:12" ht="18">
-      <c r="A106" s="9"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="8"/>
-      <c r="G106" s="9"/>
-      <c r="H106" s="9"/>
-      <c r="I106" s="9"/>
-      <c r="J106" s="9"/>
-      <c r="K106" s="9"/>
-      <c r="L106" s="9"/>
-    </row>
-    <row r="107" spans="1:12" ht="18">
-      <c r="A107" s="9"/>
-      <c r="B107" s="8"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8"/>
-      <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-      <c r="L107" s="9"/>
-    </row>
-    <row r="108" spans="1:12" ht="72" customHeight="1">
-      <c r="A108" s="9"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="9"/>
-      <c r="H108" s="9"/>
-      <c r="I108" s="9"/>
-      <c r="J108" s="9"/>
-      <c r="K108" s="9"/>
-      <c r="L108" s="9"/>
-    </row>
-    <row r="109" spans="1:12" ht="36" customHeight="1">
-      <c r="A109" s="9"/>
-      <c r="B109" s="8"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
-      <c r="F109" s="8"/>
-      <c r="G109" s="9"/>
-      <c r="H109" s="9"/>
-      <c r="I109" s="9"/>
-      <c r="J109" s="9"/>
-      <c r="K109" s="9"/>
-      <c r="L109" s="9"/>
-    </row>
-    <row r="110" spans="1:12" ht="72" customHeight="1">
-      <c r="A110" s="9"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="9"/>
-      <c r="H110" s="9"/>
-      <c r="I110" s="9"/>
-      <c r="J110" s="9"/>
-      <c r="K110" s="9"/>
-      <c r="L110" s="9"/>
-    </row>
-    <row r="111" spans="1:12" ht="36" customHeight="1">
-      <c r="A111" s="9"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="8"/>
-      <c r="G111" s="9"/>
-      <c r="H111" s="9"/>
-      <c r="I111" s="9"/>
-      <c r="J111" s="9"/>
-      <c r="K111" s="9"/>
-      <c r="L111" s="9"/>
-    </row>
-    <row r="112" spans="1:12" ht="72" customHeight="1">
-      <c r="A112" s="9"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="9"/>
-      <c r="H112" s="9"/>
-      <c r="I112" s="9"/>
-      <c r="J112" s="9"/>
-      <c r="K112" s="9"/>
-      <c r="L112" s="9"/>
-    </row>
-    <row r="113" spans="1:12" ht="72" customHeight="1">
-      <c r="A113" s="9"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="9"/>
-      <c r="H113" s="9"/>
-      <c r="I113" s="9"/>
-      <c r="J113" s="9"/>
-      <c r="K113" s="9"/>
-      <c r="L113" s="9"/>
-    </row>
-    <row r="114" spans="1:12" ht="72" customHeight="1">
-      <c r="A114" s="9"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="9"/>
-      <c r="H114" s="9"/>
-      <c r="I114" s="9"/>
-      <c r="J114" s="9"/>
-      <c r="K114" s="9"/>
-      <c r="L114" s="9"/>
-    </row>
-    <row r="115" spans="1:12" ht="72" customHeight="1">
-      <c r="A115" s="9"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="9"/>
-      <c r="H115" s="9"/>
-      <c r="I115" s="9"/>
-      <c r="J115" s="9"/>
-      <c r="K115" s="9"/>
-      <c r="L115" s="9"/>
-    </row>
-    <row r="116" spans="1:12" ht="72" customHeight="1">
-      <c r="A116" s="9"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="9"/>
-      <c r="H116" s="9"/>
-      <c r="I116" s="9"/>
-      <c r="J116" s="9"/>
-      <c r="K116" s="9"/>
-      <c r="L116" s="9"/>
-    </row>
-    <row r="117" spans="1:12" ht="72" customHeight="1">
-      <c r="A117" s="9"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="8"/>
-      <c r="F117" s="8"/>
-      <c r="G117" s="9"/>
-      <c r="H117" s="9"/>
-      <c r="I117" s="9"/>
-      <c r="J117" s="9"/>
-      <c r="K117" s="9"/>
-      <c r="L117" s="9"/>
-    </row>
-    <row r="118" spans="1:12" ht="72" customHeight="1">
-      <c r="A118" s="9"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="9"/>
-      <c r="H118" s="9"/>
-      <c r="I118" s="9"/>
-      <c r="J118" s="9"/>
-      <c r="K118" s="9"/>
-      <c r="L118" s="9"/>
-    </row>
-    <row r="119" spans="1:12">
-      <c r="A119" s="9"/>
-      <c r="B119" s="9"/>
-      <c r="C119" s="9"/>
-      <c r="D119" s="9"/>
-      <c r="E119" s="9"/>
-      <c r="F119" s="9"/>
-      <c r="G119" s="9"/>
-      <c r="H119" s="9"/>
-      <c r="I119" s="9"/>
-      <c r="J119" s="9"/>
-      <c r="K119" s="9"/>
-      <c r="L119" s="9"/>
+    <row r="61" spans="2:9" ht="17.5">
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="2:9" ht="17.5">
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="2:9" ht="17.5">
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="2:9" ht="17.5">
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="3:5" ht="17.5">
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="3:5" ht="17.5">
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="3:5" ht="17.5">
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="3:5" ht="17.5">
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="3:5" ht="17.5">
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="3:5" ht="17.5">
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="3:5" ht="17.5">
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="3:5" ht="17.5">
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="3:5" ht="17.5">
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="3:5" ht="17.5">
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="3:5" ht="17.5">
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="3:5" ht="17.5">
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="3:5" ht="17.5">
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="3:5" ht="17.5">
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="3:5" ht="17.5">
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="3:5" ht="17.5">
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="3:9" ht="17.5">
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="3:9" ht="17.5">
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+    </row>
+    <row r="83" spans="3:9" ht="17.5">
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+    </row>
+    <row r="84" spans="3:9" ht="17.5">
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="3:9" ht="17.5">
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+    </row>
+    <row r="86" spans="3:9" ht="17.5">
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+    </row>
+    <row r="87" spans="3:9" ht="17.5">
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+    </row>
+    <row r="88" spans="3:9" ht="17.5">
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+    </row>
+    <row r="89" spans="3:9" ht="17.5">
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="3:9" ht="17.5">
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+    </row>
+    <row r="91" spans="3:9" ht="17.5">
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+    </row>
+    <row r="92" spans="3:9" ht="17.5">
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+    </row>
+    <row r="93" spans="3:9" ht="17.5">
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+    </row>
+    <row r="94" spans="3:9" ht="17.5">
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+    </row>
+    <row r="95" spans="3:9" ht="17.5">
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+    </row>
+    <row r="96" spans="3:9" ht="17.5">
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="2:6" ht="108" customHeight="1">
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+    </row>
+    <row r="98" spans="2:6" ht="17.5">
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+    </row>
+    <row r="99" spans="2:6" ht="17.5">
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+    </row>
+    <row r="100" spans="2:6" ht="36" customHeight="1">
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+    </row>
+    <row r="101" spans="2:6" ht="72" customHeight="1">
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+    </row>
+    <row r="102" spans="2:6" ht="72" customHeight="1">
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+    </row>
+    <row r="103" spans="2:6" ht="36" customHeight="1">
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+    </row>
+    <row r="104" spans="2:6" ht="72" customHeight="1">
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+    </row>
+    <row r="105" spans="2:6" ht="36" customHeight="1">
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+    </row>
+    <row r="106" spans="2:6" ht="17.5">
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+    </row>
+    <row r="107" spans="2:6" ht="17.5">
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+    </row>
+    <row r="108" spans="2:6" ht="72" customHeight="1">
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+    </row>
+    <row r="109" spans="2:6" ht="36" customHeight="1">
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+    </row>
+    <row r="110" spans="2:6" ht="72" customHeight="1">
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+    </row>
+    <row r="111" spans="2:6" ht="36" customHeight="1">
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+    </row>
+    <row r="112" spans="2:6" ht="72" customHeight="1">
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+    </row>
+    <row r="113" spans="2:6" ht="72" customHeight="1">
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+    </row>
+    <row r="114" spans="2:6" ht="72" customHeight="1">
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+    </row>
+    <row r="115" spans="2:6" ht="72" customHeight="1">
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+    </row>
+    <row r="116" spans="2:6" ht="72" customHeight="1">
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+    </row>
+    <row r="117" spans="2:6" ht="72" customHeight="1">
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+    </row>
+    <row r="118" spans="2:6" ht="72" customHeight="1">
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
     <mergeCell ref="G60:I60"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="G53:I53"/>
@@ -3149,8 +2876,16 @@
     <mergeCell ref="G51:I51"/>
     <mergeCell ref="G52:I52"/>
     <mergeCell ref="G48:I48"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G43:I43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>